<commit_message>
Add and modify files for AquacultureProduction & ExportImportQuantity
</commit_message>
<xml_diff>
--- a/Country.xlsx
+++ b/Country.xlsx
@@ -1,30 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://denveru-my.sharepoint.com/personal/kexin_shang_du_edu/Documents/Pardee 2024 Winter/FAO_Fish/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://denveru-my.sharepoint.com/personal/kexin_shang_du_edu/Documents/Pardee 2024 Winter/Projects/FAO_FishStatJ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{AC94B85D-008A-4484-B872-51462EF433E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55A5B275-CF08-4819-B62B-67DB9335010E}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{AC94B85D-008A-4484-B872-51462EF433E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{806D509A-ABE3-47EE-BC9F-3D4B039B1515}"/>
   <bookViews>
-    <workbookView xWindow="29940" yWindow="4200" windowWidth="23580" windowHeight="12915" activeTab="2" xr2:uid="{3A096DD1-49D6-4DBE-9C16-F65235DFB8AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{3A096DD1-49D6-4DBE-9C16-F65235DFB8AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Production" sheetId="3" r:id="rId1"/>
     <sheet name="ExportImport" sheetId="4" r:id="rId2"/>
     <sheet name="WDI" sheetId="6" r:id="rId3"/>
-    <sheet name="WDI_Only" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
-    <sheet name="EIValue" sheetId="2" r:id="rId6"/>
+    <sheet name="AquaculturePro" sheetId="7" r:id="rId4"/>
+    <sheet name="WDI_Only" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId6"/>
+    <sheet name="EIValue" sheetId="2" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">EIValue!$A$1:$A$224</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">EIValue!$A$1:$A$224</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ExportImport!$A$1:$C$195</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Production!$A$1:$C$194</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet1!$A$1:$B$252</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$A$1:$B$252</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">WDI!$A$1:$C$189</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -48,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2586" uniqueCount="499">
   <si>
     <t>Country (Name)</t>
   </si>
@@ -1682,8 +1686,1297 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Production"/>
+      <sheetName val="ExportImport"/>
+      <sheetName val="WDI"/>
+      <sheetName val="AquaculturePro"/>
+      <sheetName val="ExportImport_Q"/>
+      <sheetName val="WDI_Only"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="EIValue"/>
+      <sheetName val="AquaPro"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Country (Name)</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Afghanistan</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Albania</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Algeria</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>American Samoa</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Andorra</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Angola</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Anguilla</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>Antigua and Barbuda</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Argentina</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Armenia</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Aruba</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>Australia</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>Austria</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>Azerbaijan</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Bahamas</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Bahrain</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Bangladesh</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Barbados</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Belarus</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Belgium</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>Belize</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Benin</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>Bermuda</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>Bhutan</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>Bolivia (Plurinat.State)</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>Bonaire/S.Eustatius/Saba</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>Bosnia and Herzegovina</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>Botswana</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Brazil</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>British Indian Ocean Ter</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>British Virgin Islands</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>Brunei Darussalam</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>Bulgaria</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>Burkina Faso</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>Burundi</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>Cabo Verde</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>Cambodia</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Cameroon</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>Canada</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>Cayman Islands</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>Central African Republic</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>Chad</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>Channel Islands</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>Chile</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>China</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>China, Hong Kong SAR</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>China, Macao SAR</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>Colombia</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>Comoros</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>Congo</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>Congo, Dem. Rep. of the</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>Cook Islands</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>Costa Rica</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>Côte d'Ivoire</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>Croatia</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57" t="str">
+            <v>Cuba</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58" t="str">
+            <v>Curaçao</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>Cyprus</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>Serbia</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>Serbia and Montenegro</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>Denmark</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>Djibouti</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>Dominica</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>Dominican Republic</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>Ecuador</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>Egypt</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>El Salvador</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>Equatorial Guinea</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>Eritrea</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71" t="str">
+            <v>Estonia</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72" t="str">
+            <v>Eswatini</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>Ethiopia</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>Ethiopia PDR</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>Falkland Is.(Malvinas)</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>FAO. 2023. Fishery and Aquaculture Statistics. Global capture production 1950-2021 (FishStatJ). In: FAO Fisheries and Aquaculture Division [online]. Rome. Updated 2023. www.fao.org/fishery/en/statistics/software/fishstatj</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>Faroe Islands</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>Fiji</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>Finland</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>France</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>French Guiana</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>French Polynesia</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>French Southern Terr</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>Gabon</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85" t="str">
+            <v>Gambia</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86" t="str">
+            <v>Georgia</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87" t="str">
+            <v>Germany</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88" t="str">
+            <v>Ghana</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89" t="str">
+            <v>Gibraltar</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90" t="str">
+            <v>Greece</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91" t="str">
+            <v>Greenland</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92" t="str">
+            <v>Grenada</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93" t="str">
+            <v>Guadeloupe</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94" t="str">
+            <v>Guam</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95" t="str">
+            <v>Guatemala</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96" t="str">
+            <v>Guinea</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97" t="str">
+            <v>Guinea-Bissau</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98" t="str">
+            <v>Guyana</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99" t="str">
+            <v>Haiti</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100" t="str">
+            <v>Honduras</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101" t="str">
+            <v>Hungary</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102" t="str">
+            <v>Iceland</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103" t="str">
+            <v>India</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104" t="str">
+            <v>Indonesia</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105" t="str">
+            <v>Iran (Islamic Rep. of)</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106" t="str">
+            <v>Iraq</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107" t="str">
+            <v>Ireland</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108" t="str">
+            <v>Isle of Man</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109" t="str">
+            <v>Israel</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110" t="str">
+            <v>Italy</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111" t="str">
+            <v>Jamaica</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112" t="str">
+            <v>Japan</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113" t="str">
+            <v>Jordan</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114" t="str">
+            <v>Kazakhstan</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115" t="str">
+            <v>Kenya</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116" t="str">
+            <v>Kiribati</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117" t="str">
+            <v>Korea, Dem. People's Rep</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118" t="str">
+            <v>Korea, Republic of</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119" t="str">
+            <v>Kuwait</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120" t="str">
+            <v>Kyrgyzstan</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121" t="str">
+            <v>Lao People's Dem. Rep.</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122" t="str">
+            <v>Latvia</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123" t="str">
+            <v>Lebanon</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124" t="str">
+            <v>Lesotho</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125" t="str">
+            <v>Liberia</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126" t="str">
+            <v>Libya</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127" t="str">
+            <v>Liechtenstein</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128" t="str">
+            <v>Lithuania</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129" t="str">
+            <v>Luxembourg</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130" t="str">
+            <v>Madagascar</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131" t="str">
+            <v>Malawi</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132" t="str">
+            <v>Malaysia</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133" t="str">
+            <v>Maldives</v>
+          </cell>
+        </row>
+        <row r="134">
+          <cell r="A134" t="str">
+            <v>Mali</v>
+          </cell>
+        </row>
+        <row r="135">
+          <cell r="A135" t="str">
+            <v>Malta</v>
+          </cell>
+        </row>
+        <row r="136">
+          <cell r="A136" t="str">
+            <v>Marshall Islands</v>
+          </cell>
+        </row>
+        <row r="137">
+          <cell r="A137" t="str">
+            <v>Martinique</v>
+          </cell>
+        </row>
+        <row r="138">
+          <cell r="A138" t="str">
+            <v>Mauritania</v>
+          </cell>
+        </row>
+        <row r="139">
+          <cell r="A139" t="str">
+            <v>Mauritius</v>
+          </cell>
+        </row>
+        <row r="140">
+          <cell r="A140" t="str">
+            <v>Mayotte</v>
+          </cell>
+        </row>
+        <row r="141">
+          <cell r="A141" t="str">
+            <v>Mexico</v>
+          </cell>
+        </row>
+        <row r="142">
+          <cell r="A142" t="str">
+            <v>Micronesia (Fed. States)</v>
+          </cell>
+        </row>
+        <row r="143">
+          <cell r="A143" t="str">
+            <v>Moldova, Republic of</v>
+          </cell>
+        </row>
+        <row r="144">
+          <cell r="A144" t="str">
+            <v>Monaco</v>
+          </cell>
+        </row>
+        <row r="145">
+          <cell r="A145" t="str">
+            <v>Mongolia</v>
+          </cell>
+        </row>
+        <row r="146">
+          <cell r="A146" t="str">
+            <v>Montenegro</v>
+          </cell>
+        </row>
+        <row r="147">
+          <cell r="A147" t="str">
+            <v>Montserrat</v>
+          </cell>
+        </row>
+        <row r="148">
+          <cell r="A148" t="str">
+            <v>Morocco</v>
+          </cell>
+        </row>
+        <row r="149">
+          <cell r="A149" t="str">
+            <v>Mozambique</v>
+          </cell>
+        </row>
+        <row r="150">
+          <cell r="A150" t="str">
+            <v>Myanmar</v>
+          </cell>
+        </row>
+        <row r="151">
+          <cell r="A151" t="str">
+            <v>Namibia</v>
+          </cell>
+        </row>
+        <row r="152">
+          <cell r="A152" t="str">
+            <v>Nauru</v>
+          </cell>
+        </row>
+        <row r="153">
+          <cell r="A153" t="str">
+            <v>Nepal</v>
+          </cell>
+        </row>
+        <row r="154">
+          <cell r="A154" t="str">
+            <v>Netherlands (Kingdom of the)</v>
+          </cell>
+        </row>
+        <row r="155">
+          <cell r="A155" t="str">
+            <v>Netherlands Antilles</v>
+          </cell>
+        </row>
+        <row r="156">
+          <cell r="A156" t="str">
+            <v>New Caledonia</v>
+          </cell>
+        </row>
+        <row r="157">
+          <cell r="A157" t="str">
+            <v>New Zealand</v>
+          </cell>
+        </row>
+        <row r="158">
+          <cell r="A158" t="str">
+            <v>Nicaragua</v>
+          </cell>
+        </row>
+        <row r="159">
+          <cell r="A159" t="str">
+            <v>Niger</v>
+          </cell>
+        </row>
+        <row r="160">
+          <cell r="A160" t="str">
+            <v>Nigeria</v>
+          </cell>
+        </row>
+        <row r="161">
+          <cell r="A161" t="str">
+            <v>Niue</v>
+          </cell>
+        </row>
+        <row r="162">
+          <cell r="A162" t="str">
+            <v>Norfolk Island</v>
+          </cell>
+        </row>
+        <row r="163">
+          <cell r="A163" t="str">
+            <v>North Macedonia</v>
+          </cell>
+        </row>
+        <row r="164">
+          <cell r="A164" t="str">
+            <v>Northern Mariana Is.</v>
+          </cell>
+        </row>
+        <row r="165">
+          <cell r="A165" t="str">
+            <v>Norway</v>
+          </cell>
+        </row>
+        <row r="166">
+          <cell r="A166" t="str">
+            <v>Oman</v>
+          </cell>
+        </row>
+        <row r="167">
+          <cell r="A167" t="str">
+            <v>Other nei</v>
+          </cell>
+        </row>
+        <row r="168">
+          <cell r="A168" t="str">
+            <v>Pakistan</v>
+          </cell>
+        </row>
+        <row r="169">
+          <cell r="A169" t="str">
+            <v>Palau</v>
+          </cell>
+        </row>
+        <row r="170">
+          <cell r="A170" t="str">
+            <v>Palestine</v>
+          </cell>
+        </row>
+        <row r="171">
+          <cell r="A171" t="str">
+            <v>Panama</v>
+          </cell>
+        </row>
+        <row r="172">
+          <cell r="A172" t="str">
+            <v>Papua New Guinea</v>
+          </cell>
+        </row>
+        <row r="173">
+          <cell r="A173" t="str">
+            <v>Paraguay</v>
+          </cell>
+        </row>
+        <row r="174">
+          <cell r="A174" t="str">
+            <v>Peru</v>
+          </cell>
+        </row>
+        <row r="175">
+          <cell r="A175" t="str">
+            <v>Philippines</v>
+          </cell>
+        </row>
+        <row r="176">
+          <cell r="A176" t="str">
+            <v>Pitcairn</v>
+          </cell>
+        </row>
+        <row r="177">
+          <cell r="A177" t="str">
+            <v>Poland</v>
+          </cell>
+        </row>
+        <row r="178">
+          <cell r="A178" t="str">
+            <v>Portugal</v>
+          </cell>
+        </row>
+        <row r="179">
+          <cell r="A179" t="str">
+            <v>Puerto Rico</v>
+          </cell>
+        </row>
+        <row r="180">
+          <cell r="A180" t="str">
+            <v>Qatar</v>
+          </cell>
+        </row>
+        <row r="181">
+          <cell r="A181" t="str">
+            <v>Réunion</v>
+          </cell>
+        </row>
+        <row r="182">
+          <cell r="A182" t="str">
+            <v>Romania</v>
+          </cell>
+        </row>
+        <row r="183">
+          <cell r="A183" t="str">
+            <v>Yugoslavia SFR</v>
+          </cell>
+        </row>
+        <row r="184">
+          <cell r="A184" t="str">
+            <v>Rwanda</v>
+          </cell>
+        </row>
+        <row r="185">
+          <cell r="A185" t="str">
+            <v>Saint Barthélemy</v>
+          </cell>
+        </row>
+        <row r="186">
+          <cell r="A186" t="str">
+            <v>Saint Helena/Asc./Trist.</v>
+          </cell>
+        </row>
+        <row r="187">
+          <cell r="A187" t="str">
+            <v>Saint Kitts and Nevis</v>
+          </cell>
+        </row>
+        <row r="188">
+          <cell r="A188" t="str">
+            <v>Saint Lucia</v>
+          </cell>
+        </row>
+        <row r="189">
+          <cell r="A189" t="str">
+            <v>Saint Vincent/Grenadines</v>
+          </cell>
+        </row>
+        <row r="190">
+          <cell r="A190" t="str">
+            <v>Saint-Martin (French)</v>
+          </cell>
+        </row>
+        <row r="191">
+          <cell r="A191" t="str">
+            <v>Samoa</v>
+          </cell>
+        </row>
+        <row r="192">
+          <cell r="A192" t="str">
+            <v>San Marino</v>
+          </cell>
+        </row>
+        <row r="193">
+          <cell r="A193" t="str">
+            <v>Sao Tome and Principe</v>
+          </cell>
+        </row>
+        <row r="194">
+          <cell r="A194" t="str">
+            <v>Saudi Arabia</v>
+          </cell>
+        </row>
+        <row r="195">
+          <cell r="A195" t="str">
+            <v>Senegal</v>
+          </cell>
+        </row>
+        <row r="196">
+          <cell r="A196" t="str">
+            <v>Russian Federation</v>
+          </cell>
+        </row>
+        <row r="197">
+          <cell r="A197" t="str">
+            <v>Un. Sov. Soc. Rep.</v>
+          </cell>
+        </row>
+        <row r="198">
+          <cell r="A198" t="str">
+            <v>Seychelles</v>
+          </cell>
+        </row>
+        <row r="199">
+          <cell r="A199" t="str">
+            <v>Sierra Leone</v>
+          </cell>
+        </row>
+        <row r="200">
+          <cell r="A200" t="str">
+            <v>Singapore</v>
+          </cell>
+        </row>
+        <row r="201">
+          <cell r="A201" t="str">
+            <v>Sint Maarten</v>
+          </cell>
+        </row>
+        <row r="202">
+          <cell r="A202" t="str">
+            <v>Slovakia</v>
+          </cell>
+        </row>
+        <row r="203">
+          <cell r="A203" t="str">
+            <v>Slovenia</v>
+          </cell>
+        </row>
+        <row r="204">
+          <cell r="A204" t="str">
+            <v>Solomon Islands</v>
+          </cell>
+        </row>
+        <row r="205">
+          <cell r="A205" t="str">
+            <v>Somalia</v>
+          </cell>
+        </row>
+        <row r="206">
+          <cell r="A206" t="str">
+            <v>South Africa</v>
+          </cell>
+        </row>
+        <row r="207">
+          <cell r="A207" t="str">
+            <v>South Sudan</v>
+          </cell>
+        </row>
+        <row r="208">
+          <cell r="A208" t="str">
+            <v>Spain</v>
+          </cell>
+        </row>
+        <row r="209">
+          <cell r="A209" t="str">
+            <v>Sri Lanka</v>
+          </cell>
+        </row>
+        <row r="210">
+          <cell r="A210" t="str">
+            <v>St. Pierre and Miquelon</v>
+          </cell>
+        </row>
+        <row r="211">
+          <cell r="A211" t="str">
+            <v>Czechia</v>
+          </cell>
+        </row>
+        <row r="212">
+          <cell r="A212" t="str">
+            <v>Czechoslovakia</v>
+          </cell>
+        </row>
+        <row r="213">
+          <cell r="A213" t="str">
+            <v>Suriname</v>
+          </cell>
+        </row>
+        <row r="214">
+          <cell r="A214" t="str">
+            <v>Svalbard and Jan Mayen</v>
+          </cell>
+        </row>
+        <row r="215">
+          <cell r="A215" t="str">
+            <v>Sweden</v>
+          </cell>
+        </row>
+        <row r="216">
+          <cell r="A216" t="str">
+            <v>Switzerland</v>
+          </cell>
+        </row>
+        <row r="217">
+          <cell r="A217" t="str">
+            <v>Syrian Arab Republic</v>
+          </cell>
+        </row>
+        <row r="218">
+          <cell r="A218" t="str">
+            <v>Taiwan Province of China</v>
+          </cell>
+        </row>
+        <row r="219">
+          <cell r="A219" t="str">
+            <v>Tajikistan</v>
+          </cell>
+        </row>
+        <row r="220">
+          <cell r="A220" t="str">
+            <v>Tanzania, United Rep. of</v>
+          </cell>
+        </row>
+        <row r="221">
+          <cell r="A221" t="str">
+            <v>Thailand</v>
+          </cell>
+        </row>
+        <row r="222">
+          <cell r="A222" t="str">
+            <v>Timor-Leste</v>
+          </cell>
+        </row>
+        <row r="223">
+          <cell r="A223" t="str">
+            <v>Togo</v>
+          </cell>
+        </row>
+        <row r="224">
+          <cell r="A224" t="str">
+            <v>Tokelau</v>
+          </cell>
+        </row>
+        <row r="225">
+          <cell r="A225" t="str">
+            <v>Tonga</v>
+          </cell>
+        </row>
+        <row r="226">
+          <cell r="A226" t="str">
+            <v>Totals - Number</v>
+          </cell>
+        </row>
+        <row r="227">
+          <cell r="A227" t="str">
+            <v>Totals - Tonnes - live weight</v>
+          </cell>
+        </row>
+        <row r="228">
+          <cell r="A228" t="str">
+            <v>Trinidad and Tobago</v>
+          </cell>
+        </row>
+        <row r="229">
+          <cell r="A229" t="str">
+            <v>Tunisia</v>
+          </cell>
+        </row>
+        <row r="230">
+          <cell r="A230" t="str">
+            <v>Türkiye</v>
+          </cell>
+        </row>
+        <row r="231">
+          <cell r="A231" t="str">
+            <v>Turkmenistan</v>
+          </cell>
+        </row>
+        <row r="232">
+          <cell r="A232" t="str">
+            <v>Turks and Caicos Is.</v>
+          </cell>
+        </row>
+        <row r="233">
+          <cell r="A233" t="str">
+            <v>Tuvalu</v>
+          </cell>
+        </row>
+        <row r="234">
+          <cell r="A234" t="str">
+            <v>Uganda</v>
+          </cell>
+        </row>
+        <row r="235">
+          <cell r="A235" t="str">
+            <v>Ukraine</v>
+          </cell>
+        </row>
+        <row r="236">
+          <cell r="A236" t="str">
+            <v>Sudan</v>
+          </cell>
+        </row>
+        <row r="237">
+          <cell r="A237" t="str">
+            <v>United Arab Emirates</v>
+          </cell>
+        </row>
+        <row r="238">
+          <cell r="A238" t="str">
+            <v>United Kingdom</v>
+          </cell>
+        </row>
+        <row r="239">
+          <cell r="A239" t="str">
+            <v>United Republic of Tanzania, Zanzibar</v>
+          </cell>
+        </row>
+        <row r="240">
+          <cell r="A240" t="str">
+            <v>United States of America</v>
+          </cell>
+        </row>
+        <row r="241">
+          <cell r="A241" t="str">
+            <v>Uruguay</v>
+          </cell>
+        </row>
+        <row r="242">
+          <cell r="A242" t="str">
+            <v>US Virgin Islands</v>
+          </cell>
+        </row>
+        <row r="243">
+          <cell r="A243" t="str">
+            <v>Uzbekistan</v>
+          </cell>
+        </row>
+        <row r="244">
+          <cell r="A244" t="str">
+            <v>Vanuatu</v>
+          </cell>
+        </row>
+        <row r="245">
+          <cell r="A245" t="str">
+            <v>Venezuela (Boliv Rep of)</v>
+          </cell>
+        </row>
+        <row r="246">
+          <cell r="A246" t="str">
+            <v>Viet Nam</v>
+          </cell>
+        </row>
+        <row r="247">
+          <cell r="A247" t="str">
+            <v>Wallis and Futuna Is.</v>
+          </cell>
+        </row>
+        <row r="248">
+          <cell r="A248" t="str">
+            <v>Western Sahara</v>
+          </cell>
+        </row>
+        <row r="249">
+          <cell r="A249" t="str">
+            <v>Yemen</v>
+          </cell>
+        </row>
+        <row r="250">
+          <cell r="A250" t="str">
+            <v>Sudan (former)</v>
+          </cell>
+        </row>
+        <row r="251">
+          <cell r="A251" t="str">
+            <v>Zambia</v>
+          </cell>
+        </row>
+        <row r="252">
+          <cell r="A252" t="str">
+            <v>Zimbabwe</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6486,7 +7779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571B96FD-504C-4ABF-8EE0-3B6600A80015}">
   <dimension ref="A1:C189"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -8738,6 +10031,2238 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E62C76-D463-44F4-8E19-F3353B166DCF}">
+  <dimension ref="A1:C194"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="L184" sqref="L184"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>270</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20" t="s">
+        <v>276</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>277</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" t="s">
+        <v>278</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>279</v>
+      </c>
+      <c r="C23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>280</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>281</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" t="s">
+        <v>282</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>283</v>
+      </c>
+      <c r="C27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" t="s">
+        <v>284</v>
+      </c>
+      <c r="C28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
+        <v>286</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
+        <v>288</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>289</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="s">
+        <v>290</v>
+      </c>
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>291</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" t="s">
+        <v>292</v>
+      </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>293</v>
+      </c>
+      <c r="C37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>294</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>295</v>
+      </c>
+      <c r="B39" t="s">
+        <v>296</v>
+      </c>
+      <c r="C39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>297</v>
+      </c>
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>298</v>
+      </c>
+      <c r="B41" t="s">
+        <v>299</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>300</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>301</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
+        <v>302</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B45" t="s">
+        <v>304</v>
+      </c>
+      <c r="C45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B46" t="s">
+        <v>304</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>305</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" t="s">
+        <v>306</v>
+      </c>
+      <c r="C48" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" t="s">
+        <v>307</v>
+      </c>
+      <c r="C49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" t="s">
+        <v>308</v>
+      </c>
+      <c r="C50" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="s">
+        <v>309</v>
+      </c>
+      <c r="C51" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" t="s">
+        <v>310</v>
+      </c>
+      <c r="C52" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" t="s">
+        <v>311</v>
+      </c>
+      <c r="C53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" t="s">
+        <v>312</v>
+      </c>
+      <c r="C54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" t="s">
+        <v>313</v>
+      </c>
+      <c r="C55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>71</v>
+      </c>
+      <c r="B56" t="s">
+        <v>314</v>
+      </c>
+      <c r="C56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" t="s">
+        <v>316</v>
+      </c>
+      <c r="C58" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>317</v>
+      </c>
+      <c r="C59" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" t="s">
+        <v>318</v>
+      </c>
+      <c r="C60" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B61" t="s">
+        <v>319</v>
+      </c>
+      <c r="C61" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>82</v>
+      </c>
+      <c r="B62" t="s">
+        <v>320</v>
+      </c>
+      <c r="C62" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>83</v>
+      </c>
+      <c r="B63" t="s">
+        <v>321</v>
+      </c>
+      <c r="C63" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" t="s">
+        <v>322</v>
+      </c>
+      <c r="C64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>85</v>
+      </c>
+      <c r="B65" t="s">
+        <v>323</v>
+      </c>
+      <c r="C65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" t="s">
+        <v>324</v>
+      </c>
+      <c r="C66" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" t="s">
+        <v>325</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>92</v>
+      </c>
+      <c r="B68" t="s">
+        <v>326</v>
+      </c>
+      <c r="C68" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>93</v>
+      </c>
+      <c r="B69" t="s">
+        <v>327</v>
+      </c>
+      <c r="C69" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>328</v>
+      </c>
+      <c r="B70" t="s">
+        <v>329</v>
+      </c>
+      <c r="C70" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" t="s">
+        <v>330</v>
+      </c>
+      <c r="C71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" t="s">
+        <v>331</v>
+      </c>
+      <c r="C72" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>97</v>
+      </c>
+      <c r="B73" t="s">
+        <v>332</v>
+      </c>
+      <c r="C73" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>333</v>
+      </c>
+      <c r="B74" t="s">
+        <v>334</v>
+      </c>
+      <c r="C74" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" t="s">
+        <v>335</v>
+      </c>
+      <c r="C75" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" t="s">
+        <v>336</v>
+      </c>
+      <c r="C76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" t="s">
+        <v>337</v>
+      </c>
+      <c r="C77" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" t="s">
+        <v>338</v>
+      </c>
+      <c r="C78" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>339</v>
+      </c>
+      <c r="B79" t="s">
+        <v>340</v>
+      </c>
+      <c r="C79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" t="s">
+        <v>341</v>
+      </c>
+      <c r="C80" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" t="s">
+        <v>342</v>
+      </c>
+      <c r="C81" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>106</v>
+      </c>
+      <c r="B82" t="s">
+        <v>343</v>
+      </c>
+      <c r="C82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" t="s">
+        <v>344</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>108</v>
+      </c>
+      <c r="B84" t="s">
+        <v>345</v>
+      </c>
+      <c r="C84" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>109</v>
+      </c>
+      <c r="B85" t="s">
+        <v>346</v>
+      </c>
+      <c r="C85" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>110</v>
+      </c>
+      <c r="B86" t="s">
+        <v>347</v>
+      </c>
+      <c r="C86" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>111</v>
+      </c>
+      <c r="B87" t="s">
+        <v>348</v>
+      </c>
+      <c r="C87" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88" t="s">
+        <v>349</v>
+      </c>
+      <c r="C88" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>113</v>
+      </c>
+      <c r="B89" t="s">
+        <v>350</v>
+      </c>
+      <c r="C89" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>351</v>
+      </c>
+      <c r="B90" t="s">
+        <v>352</v>
+      </c>
+      <c r="C90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>115</v>
+      </c>
+      <c r="B91" t="s">
+        <v>353</v>
+      </c>
+      <c r="C91" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>354</v>
+      </c>
+      <c r="B92" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" t="s">
+        <v>356</v>
+      </c>
+      <c r="C93" t="str">
+        <f>VLOOKUP(A93,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Kuwait</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" t="s">
+        <v>357</v>
+      </c>
+      <c r="C94" t="str">
+        <f>VLOOKUP(A94,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Kyrgyzstan</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>358</v>
+      </c>
+      <c r="B95" t="s">
+        <v>359</v>
+      </c>
+      <c r="C95" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" t="s">
+        <v>360</v>
+      </c>
+      <c r="C96" t="str">
+        <f>VLOOKUP(A96,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Latvia</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" t="s">
+        <v>361</v>
+      </c>
+      <c r="C97" t="str">
+        <f>VLOOKUP(A97,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Lebanon</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>121</v>
+      </c>
+      <c r="B98" t="s">
+        <v>362</v>
+      </c>
+      <c r="C98" t="str">
+        <f>VLOOKUP(A98,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Lesotho</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>122</v>
+      </c>
+      <c r="B99" t="s">
+        <v>363</v>
+      </c>
+      <c r="C99" t="str">
+        <f>VLOOKUP(A99,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Liberia</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" t="s">
+        <v>364</v>
+      </c>
+      <c r="C100" t="str">
+        <f>VLOOKUP(A100,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Libya</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>125</v>
+      </c>
+      <c r="B101" t="s">
+        <v>365</v>
+      </c>
+      <c r="C101" t="str">
+        <f>VLOOKUP(A101,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Lithuania</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>126</v>
+      </c>
+      <c r="B102" t="s">
+        <v>366</v>
+      </c>
+      <c r="C102" t="str">
+        <f>VLOOKUP(A102,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Luxembourg</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>367</v>
+      </c>
+      <c r="B103" t="s">
+        <v>368</v>
+      </c>
+      <c r="C103" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>127</v>
+      </c>
+      <c r="B104" t="s">
+        <v>369</v>
+      </c>
+      <c r="C104" t="str">
+        <f>VLOOKUP(A104,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Madagascar</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" t="s">
+        <v>370</v>
+      </c>
+      <c r="C105" t="str">
+        <f>VLOOKUP(A105,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Malawi</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>129</v>
+      </c>
+      <c r="B106" t="s">
+        <v>371</v>
+      </c>
+      <c r="C106" t="str">
+        <f>VLOOKUP(A106,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Malaysia</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" t="s">
+        <v>372</v>
+      </c>
+      <c r="C107" t="str">
+        <f>VLOOKUP(A107,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Maldives</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>131</v>
+      </c>
+      <c r="B108" t="s">
+        <v>373</v>
+      </c>
+      <c r="C108" t="str">
+        <f>VLOOKUP(A108,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Mali</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>132</v>
+      </c>
+      <c r="B109" t="s">
+        <v>374</v>
+      </c>
+      <c r="C109" t="str">
+        <f>VLOOKUP(A109,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Malta</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>135</v>
+      </c>
+      <c r="B110" t="s">
+        <v>375</v>
+      </c>
+      <c r="C110" t="str">
+        <f>VLOOKUP(A110,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Mauritania</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>136</v>
+      </c>
+      <c r="B111" t="s">
+        <v>376</v>
+      </c>
+      <c r="C111" t="str">
+        <f>VLOOKUP(A111,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Mauritius</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>138</v>
+      </c>
+      <c r="B112" t="s">
+        <v>377</v>
+      </c>
+      <c r="C112" t="str">
+        <f>VLOOKUP(A112,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Mexico</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>378</v>
+      </c>
+      <c r="B113" t="s">
+        <v>379</v>
+      </c>
+      <c r="C113" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>140</v>
+      </c>
+      <c r="B114" t="s">
+        <v>380</v>
+      </c>
+      <c r="C114" t="str">
+        <f>VLOOKUP(A114,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Moldova, Republic of</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>142</v>
+      </c>
+      <c r="B115" t="s">
+        <v>381</v>
+      </c>
+      <c r="C115" t="str">
+        <f>VLOOKUP(A115,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Mongolia</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>143</v>
+      </c>
+      <c r="B116" t="s">
+        <v>382</v>
+      </c>
+      <c r="C116" t="str">
+        <f>VLOOKUP(A116,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Montenegro</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>145</v>
+      </c>
+      <c r="B117" t="s">
+        <v>383</v>
+      </c>
+      <c r="C117" t="str">
+        <f>VLOOKUP(A117,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Morocco</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>146</v>
+      </c>
+      <c r="B118" t="s">
+        <v>384</v>
+      </c>
+      <c r="C118" t="str">
+        <f>VLOOKUP(A118,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Mozambique</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>147</v>
+      </c>
+      <c r="B119" t="s">
+        <v>385</v>
+      </c>
+      <c r="C119" t="str">
+        <f>VLOOKUP(A119,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Myanmar</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>148</v>
+      </c>
+      <c r="B120" t="s">
+        <v>386</v>
+      </c>
+      <c r="C120" t="str">
+        <f>VLOOKUP(A120,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Namibia</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>150</v>
+      </c>
+      <c r="B121" t="s">
+        <v>387</v>
+      </c>
+      <c r="C121" t="str">
+        <f>VLOOKUP(A121,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Nepal</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>388</v>
+      </c>
+      <c r="B122" t="s">
+        <v>389</v>
+      </c>
+      <c r="C122" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A123" t="s">
+        <v>154</v>
+      </c>
+      <c r="B123" t="s">
+        <v>390</v>
+      </c>
+      <c r="C123" t="str">
+        <f>VLOOKUP(A123,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>New Zealand</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A124" t="s">
+        <v>155</v>
+      </c>
+      <c r="B124" t="s">
+        <v>391</v>
+      </c>
+      <c r="C124" t="str">
+        <f>VLOOKUP(A124,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Nicaragua</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A125" t="s">
+        <v>156</v>
+      </c>
+      <c r="B125" t="s">
+        <v>392</v>
+      </c>
+      <c r="C125" t="str">
+        <f>VLOOKUP(A125,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Niger</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A126" t="s">
+        <v>157</v>
+      </c>
+      <c r="B126" t="s">
+        <v>393</v>
+      </c>
+      <c r="C126" t="str">
+        <f>VLOOKUP(A126,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Nigeria</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A127" t="s">
+        <v>162</v>
+      </c>
+      <c r="B127" t="s">
+        <v>394</v>
+      </c>
+      <c r="C127" t="str">
+        <f>VLOOKUP(A127,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Norway</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A128" t="s">
+        <v>163</v>
+      </c>
+      <c r="B128" t="s">
+        <v>395</v>
+      </c>
+      <c r="C128" t="str">
+        <f>VLOOKUP(A128,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Oman</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A129" t="s">
+        <v>165</v>
+      </c>
+      <c r="B129" t="s">
+        <v>396</v>
+      </c>
+      <c r="C129" t="str">
+        <f>VLOOKUP(A129,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Pakistan</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A130" t="s">
+        <v>167</v>
+      </c>
+      <c r="B130" t="s">
+        <v>397</v>
+      </c>
+      <c r="C130" t="str">
+        <f>VLOOKUP(A130,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Palestine</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A131" t="s">
+        <v>168</v>
+      </c>
+      <c r="B131" t="s">
+        <v>398</v>
+      </c>
+      <c r="C131" t="str">
+        <f>VLOOKUP(A131,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Panama</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A132" t="s">
+        <v>169</v>
+      </c>
+      <c r="B132" t="s">
+        <v>399</v>
+      </c>
+      <c r="C132" t="str">
+        <f>VLOOKUP(A132,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Papua New Guinea</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
+        <v>170</v>
+      </c>
+      <c r="B133" t="s">
+        <v>400</v>
+      </c>
+      <c r="C133" t="str">
+        <f>VLOOKUP(A133,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Paraguay</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A134" t="s">
+        <v>171</v>
+      </c>
+      <c r="B134" t="s">
+        <v>401</v>
+      </c>
+      <c r="C134" t="str">
+        <f>VLOOKUP(A134,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Peru</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A135" t="s">
+        <v>172</v>
+      </c>
+      <c r="B135" t="s">
+        <v>402</v>
+      </c>
+      <c r="C135" t="str">
+        <f>VLOOKUP(A135,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Philippines</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>174</v>
+      </c>
+      <c r="B136" t="s">
+        <v>403</v>
+      </c>
+      <c r="C136" t="str">
+        <f>VLOOKUP(A136,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Poland</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>175</v>
+      </c>
+      <c r="B137" t="s">
+        <v>404</v>
+      </c>
+      <c r="C137" t="str">
+        <f>VLOOKUP(A137,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Portugal</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>176</v>
+      </c>
+      <c r="B138" t="s">
+        <v>405</v>
+      </c>
+      <c r="C138" t="str">
+        <f>VLOOKUP(A138,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Puerto Rico</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>177</v>
+      </c>
+      <c r="B139" t="s">
+        <v>406</v>
+      </c>
+      <c r="C139" t="str">
+        <f>VLOOKUP(A139,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Qatar</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>178</v>
+      </c>
+      <c r="B140" t="s">
+        <v>407</v>
+      </c>
+      <c r="C140" t="str">
+        <f>VLOOKUP(A140,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Romania</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A141" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B141" t="s">
+        <v>408</v>
+      </c>
+      <c r="C141" t="str">
+        <f>VLOOKUP(A141,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Russian Federation</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A142" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="B142" t="s">
+        <v>408</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>180</v>
+      </c>
+      <c r="B143" t="s">
+        <v>409</v>
+      </c>
+      <c r="C143" t="str">
+        <f>VLOOKUP(A143,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Rwanda</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>410</v>
+      </c>
+      <c r="B144" t="s">
+        <v>411</v>
+      </c>
+      <c r="C144" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>188</v>
+      </c>
+      <c r="B145" t="s">
+        <v>412</v>
+      </c>
+      <c r="C145" t="str">
+        <f>VLOOKUP(A145,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Samoa</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>190</v>
+      </c>
+      <c r="B146" t="s">
+        <v>413</v>
+      </c>
+      <c r="C146" t="str">
+        <f>VLOOKUP(A146,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Sao Tome and Principe</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>191</v>
+      </c>
+      <c r="B147" t="s">
+        <v>414</v>
+      </c>
+      <c r="C147" t="str">
+        <f>VLOOKUP(A147,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Saudi Arabia</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>192</v>
+      </c>
+      <c r="B148" t="s">
+        <v>415</v>
+      </c>
+      <c r="C148" t="str">
+        <f>VLOOKUP(A148,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Senegal</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A149" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B149" t="s">
+        <v>416</v>
+      </c>
+      <c r="C149" t="str">
+        <f>VLOOKUP(A149,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Serbia</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A150" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B150" t="s">
+        <v>416</v>
+      </c>
+      <c r="C150" s="10" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A151" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="B151" t="s">
+        <v>416</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>195</v>
+      </c>
+      <c r="B152" t="s">
+        <v>417</v>
+      </c>
+      <c r="C152" t="str">
+        <f>VLOOKUP(A152,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Seychelles</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>196</v>
+      </c>
+      <c r="B153" t="s">
+        <v>418</v>
+      </c>
+      <c r="C153" t="str">
+        <f>VLOOKUP(A153,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Sierra Leone</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>197</v>
+      </c>
+      <c r="B154" t="s">
+        <v>419</v>
+      </c>
+      <c r="C154" t="str">
+        <f>VLOOKUP(A154,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Singapore</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>199</v>
+      </c>
+      <c r="B155" t="s">
+        <v>420</v>
+      </c>
+      <c r="C155" t="str">
+        <f>VLOOKUP(A155,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Slovakia</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>200</v>
+      </c>
+      <c r="B156" t="s">
+        <v>421</v>
+      </c>
+      <c r="C156" t="str">
+        <f>VLOOKUP(A156,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Slovenia</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>201</v>
+      </c>
+      <c r="B157" t="s">
+        <v>422</v>
+      </c>
+      <c r="C157" t="str">
+        <f>VLOOKUP(A157,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Solomon Islands</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>202</v>
+      </c>
+      <c r="B158" t="s">
+        <v>423</v>
+      </c>
+      <c r="C158" t="str">
+        <f>VLOOKUP(A158,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Somalia</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>203</v>
+      </c>
+      <c r="B159" t="s">
+        <v>424</v>
+      </c>
+      <c r="C159" t="str">
+        <f>VLOOKUP(A159,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>South Africa</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>205</v>
+      </c>
+      <c r="B160" t="s">
+        <v>425</v>
+      </c>
+      <c r="C160" t="str">
+        <f>VLOOKUP(A160,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Spain</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>206</v>
+      </c>
+      <c r="B161" t="s">
+        <v>426</v>
+      </c>
+      <c r="C161" t="str">
+        <f>VLOOKUP(A161,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Sri Lanka</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>427</v>
+      </c>
+      <c r="B162" t="s">
+        <v>428</v>
+      </c>
+      <c r="C162" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>429</v>
+      </c>
+      <c r="B163" t="s">
+        <v>430</v>
+      </c>
+      <c r="C163" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A164" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B164" t="s">
+        <v>431</v>
+      </c>
+      <c r="C164" t="str">
+        <f>VLOOKUP(A164,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Sudan</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A165" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B165" t="s">
+        <v>431</v>
+      </c>
+      <c r="C165" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>432</v>
+      </c>
+      <c r="B166" t="s">
+        <v>433</v>
+      </c>
+      <c r="C166" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>210</v>
+      </c>
+      <c r="B167" t="s">
+        <v>434</v>
+      </c>
+      <c r="C167" t="str">
+        <f>VLOOKUP(A167,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Suriname</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>212</v>
+      </c>
+      <c r="B168" t="s">
+        <v>435</v>
+      </c>
+      <c r="C168" t="str">
+        <f>VLOOKUP(A168,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Sweden</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>213</v>
+      </c>
+      <c r="B169" t="s">
+        <v>436</v>
+      </c>
+      <c r="C169" t="str">
+        <f>VLOOKUP(A169,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Switzerland</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>214</v>
+      </c>
+      <c r="B170" t="s">
+        <v>437</v>
+      </c>
+      <c r="C170" t="str">
+        <f>VLOOKUP(A170,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Syrian Arab Republic</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>438</v>
+      </c>
+      <c r="B171" t="s">
+        <v>439</v>
+      </c>
+      <c r="C171" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>216</v>
+      </c>
+      <c r="B172" t="s">
+        <v>440</v>
+      </c>
+      <c r="C172" t="str">
+        <f>VLOOKUP(A172,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Tajikistan</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A173" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="B173" t="s">
+        <v>442</v>
+      </c>
+      <c r="C173" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>218</v>
+      </c>
+      <c r="B174" t="s">
+        <v>443</v>
+      </c>
+      <c r="C174" t="str">
+        <f>VLOOKUP(A174,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Thailand</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>219</v>
+      </c>
+      <c r="B175" t="s">
+        <v>444</v>
+      </c>
+      <c r="C175" t="str">
+        <f>VLOOKUP(A175,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Timor-Leste</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>220</v>
+      </c>
+      <c r="B176" t="s">
+        <v>445</v>
+      </c>
+      <c r="C176" t="str">
+        <f>VLOOKUP(A176,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Togo</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>222</v>
+      </c>
+      <c r="B177" t="s">
+        <v>446</v>
+      </c>
+      <c r="C177" t="str">
+        <f>VLOOKUP(A177,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Tonga</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>223</v>
+      </c>
+      <c r="B178" t="s">
+        <v>447</v>
+      </c>
+      <c r="C178" t="str">
+        <f>VLOOKUP(A178,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Trinidad and Tobago</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>224</v>
+      </c>
+      <c r="B179" t="s">
+        <v>448</v>
+      </c>
+      <c r="C179" t="str">
+        <f>VLOOKUP(A179,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Tunisia</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>449</v>
+      </c>
+      <c r="B180" t="s">
+        <v>450</v>
+      </c>
+      <c r="C180" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>225</v>
+      </c>
+      <c r="B181" t="s">
+        <v>451</v>
+      </c>
+      <c r="C181" t="str">
+        <f>VLOOKUP(A181,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Turkmenistan</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>230</v>
+      </c>
+      <c r="B182" t="s">
+        <v>452</v>
+      </c>
+      <c r="C182" t="str">
+        <f>VLOOKUP(A182,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Uganda</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>231</v>
+      </c>
+      <c r="B183" t="s">
+        <v>453</v>
+      </c>
+      <c r="C183" t="str">
+        <f>VLOOKUP(A183,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Ukraine</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>233</v>
+      </c>
+      <c r="B184" t="s">
+        <v>454</v>
+      </c>
+      <c r="C184" t="str">
+        <f>VLOOKUP(A184,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>United Arab Emirates</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>234</v>
+      </c>
+      <c r="B185" t="s">
+        <v>455</v>
+      </c>
+      <c r="C185" t="str">
+        <f>VLOOKUP(A185,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>United Kingdom</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>236</v>
+      </c>
+      <c r="B186" t="s">
+        <v>456</v>
+      </c>
+      <c r="C186" t="str">
+        <f>VLOOKUP(A186,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>United States of America</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>237</v>
+      </c>
+      <c r="B187" t="s">
+        <v>457</v>
+      </c>
+      <c r="C187" t="str">
+        <f>VLOOKUP(A187,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Uruguay</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>238</v>
+      </c>
+      <c r="B188" t="s">
+        <v>458</v>
+      </c>
+      <c r="C188" t="str">
+        <f>VLOOKUP(A188,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Uzbekistan</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>239</v>
+      </c>
+      <c r="B189" t="s">
+        <v>459</v>
+      </c>
+      <c r="C189" t="str">
+        <f>VLOOKUP(A189,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Vanuatu</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>460</v>
+      </c>
+      <c r="B190" t="s">
+        <v>461</v>
+      </c>
+      <c r="C190" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>241</v>
+      </c>
+      <c r="B191" t="s">
+        <v>462</v>
+      </c>
+      <c r="C191" t="str">
+        <f>VLOOKUP(A191,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Viet Nam</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>244</v>
+      </c>
+      <c r="B192" t="s">
+        <v>463</v>
+      </c>
+      <c r="C192" t="str">
+        <f>VLOOKUP(A192,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Yemen</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>246</v>
+      </c>
+      <c r="B193" t="s">
+        <v>464</v>
+      </c>
+      <c r="C193" t="str">
+        <f>VLOOKUP(A193,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Zambia</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>247</v>
+      </c>
+      <c r="B194" t="s">
+        <v>465</v>
+      </c>
+      <c r="C194" t="str">
+        <f>VLOOKUP(A194,[1]Sheet1!$A$1:$A$252,1,0)</f>
+        <v>Zimbabwe</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7515DDD9-52E6-4594-AF84-B57A90D7591E}">
   <dimension ref="A1:A218"/>
   <sheetViews>
@@ -9842,7 +13367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D942B54E-A52B-42D7-8D96-DBA393983722}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:C252"/>
@@ -12166,7 +15691,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B1A8CA-7690-491A-8C7D-91BBC75E72DD}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:A224"/>

</xml_diff>